<commit_message>
TimeTracking  - end of the day
</commit_message>
<xml_diff>
--- a/TimeTracker.xlsx
+++ b/TimeTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasmitala/Documents/School/DISS-2023-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A62DF5-497F-2F44-BEBB-20835D64E48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621F3EC9-F9C8-7E41-9657-471DCA4FDA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{B332D0A3-3666-4C42-9630-9D737949A97C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>S2 - nie všetko</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Utorok 23.4</t>
+  </si>
+  <si>
+    <t>Streda 24.4</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B49A39C-1CA7-3B43-A241-07BEA68B7549}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +444,7 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -460,70 +463,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
-        <f>1+3</f>
+      <c r="E3" s="1">
+        <f>SUM(F3:G3)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUM(F4:J4)</f>
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f>SUM(A2:A12)</f>
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f>SUM(E2:E12)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Stat - added last stat
</commit_message>
<xml_diff>
--- a/TimeTracker.xlsx
+++ b/TimeTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasmitala/Documents/School/DISS-2023-2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WinSubory\Dokumenty\Škola\Vysoká škola\8 Semester\DISS\DISS-2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1654819-A843-AE40-9802-6405CE685BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B49C37-CEFF-4285-9734-65CEA8C9678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{B332D0A3-3666-4C42-9630-9D737949A97C}"/>
+    <workbookView xWindow="26295" yWindow="1800" windowWidth="21810" windowHeight="15315" xr2:uid="{B332D0A3-3666-4C42-9630-9D737949A97C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>S2 - nie všetko</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Utorok 30.4</t>
+  </si>
+  <si>
+    <t>Streda 1.5</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,7 +147,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,15 +466,15 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -490,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -508,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -529,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -540,7 +543,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -551,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -569,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -587,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -608,42 +611,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f>SUM(F10:I10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(F11:I11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>SUM(A2:A12)</f>
         <v>82</v>
       </c>
       <c r="E13">
         <f>SUM(E2:E12)</f>
-        <v>44.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>

</xml_diff>